<commit_message>
Ajust with data resoruces 20202
</commit_message>
<xml_diff>
--- a/addicional_data/Indicaciones-Mapeos_2023.xlsx
+++ b/addicional_data/Indicaciones-Mapeos_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Cristian_data\Humboldt\Git\Unif_biological_data_-set16-\addicional_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3812BE7E-7FB7-4DBD-A8EE-2C247ABDE7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3B4D65-B857-40D0-9A1B-146F1FE6EA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33660" yWindow="600" windowWidth="21600" windowHeight="11385" tabRatio="774" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="774" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="blank2keep" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,25 @@
     <sheet name="oficial_data" sheetId="12" r:id="rId4"/>
     <sheet name="Definitions" sheetId="15" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="450">
   <si>
     <t>lon</t>
   </si>
@@ -1924,11 +1937,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2267,9 +2280,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IE14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X12" sqref="X12"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15"/>
@@ -2451,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>251</v>
       </c>
       <c r="D3" t="s">
         <v>70</v>
@@ -2464,6 +2477,9 @@
       </c>
       <c r="G3" t="s">
         <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>26</v>
@@ -2480,6 +2496,9 @@
       </c>
       <c r="N3" s="8" t="s">
         <v>21</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="Y3" t="s">
         <v>62</v>
@@ -2540,7 +2559,7 @@
       <c r="G4" t="s">
         <v>161</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="4" t="s">
         <v>160</v>
       </c>
       <c r="I4" t="s">
@@ -2557,6 +2576,9 @@
       </c>
       <c r="N4" t="s">
         <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>8</v>
       </c>
       <c r="P4" t="s">
         <v>158</v>
@@ -4117,7 +4139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -4727,10 +4749,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D3B1B9-00CF-4FB8-9D54-860845AB5DAC}">
-  <dimension ref="B1:Q32"/>
+  <dimension ref="B1:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4758,22 +4780,22 @@
       <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
     </row>
     <row r="3" spans="2:17">
       <c r="B3" s="8" t="s">
@@ -4782,176 +4804,176 @@
       <c r="C3" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="2:17">
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="2:17">
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
     </row>
     <row r="6" spans="2:17">
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="2:17">
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
     </row>
     <row r="8" spans="2:17">
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="2:17">
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="2:17">
       <c r="B10" s="8"/>
       <c r="C10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
     </row>
     <row r="11" spans="2:17">
       <c r="B11" s="8" t="s">
@@ -4960,22 +4982,22 @@
       <c r="C11" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
     </row>
     <row r="12" spans="2:17">
       <c r="B12" s="8" t="s">
@@ -4984,22 +5006,22 @@
       <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
     </row>
     <row r="13" spans="2:17">
       <c r="B13" s="8" t="s">
@@ -5008,22 +5030,22 @@
       <c r="C13" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
     </row>
     <row r="14" spans="2:17" ht="26.25" customHeight="1">
       <c r="B14" s="8" t="s">
@@ -5032,22 +5054,22 @@
       <c r="C14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="2:17">
       <c r="B15" s="8" t="s">
@@ -5056,22 +5078,22 @@
       <c r="C15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
     </row>
     <row r="16" spans="2:17">
       <c r="B16" s="8" t="s">
@@ -5080,22 +5102,22 @@
       <c r="C16" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
     </row>
     <row r="17" spans="2:17">
       <c r="B17" s="8" t="s">
@@ -5104,22 +5126,22 @@
       <c r="C17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
     </row>
     <row r="18" spans="2:17" ht="27.75" customHeight="1">
       <c r="B18" s="8" t="s">
@@ -5128,22 +5150,22 @@
       <c r="C18" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
     </row>
     <row r="19" spans="2:17">
       <c r="B19" s="8" t="s">
@@ -5152,22 +5174,22 @@
       <c r="C19" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
     </row>
     <row r="20" spans="2:17">
       <c r="B20" s="8" t="s">
@@ -5176,22 +5198,22 @@
       <c r="C20" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
     </row>
     <row r="21" spans="2:17">
       <c r="B21" s="8" t="s">
@@ -5200,22 +5222,22 @@
       <c r="C21" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="8" t="s">
@@ -5224,22 +5246,22 @@
       <c r="C22" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
     </row>
     <row r="23" spans="2:17">
       <c r="B23" s="8" t="s">
@@ -5248,22 +5270,22 @@
       <c r="C23" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
     </row>
     <row r="24" spans="2:17" ht="27" customHeight="1">
       <c r="B24" s="8" t="s">
@@ -5272,22 +5294,22 @@
       <c r="C24" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>428</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
     </row>
     <row r="25" spans="2:17">
       <c r="B25" s="8" t="s">
@@ -5296,22 +5318,22 @@
       <c r="C25" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="2:17">
       <c r="B26" s="8" t="s">
@@ -5320,22 +5342,22 @@
       <c r="C26" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
     </row>
     <row r="27" spans="2:17">
       <c r="B27" s="8" t="s">
@@ -5344,22 +5366,22 @@
       <c r="C27" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
     </row>
     <row r="28" spans="2:17">
       <c r="B28" s="8" t="s">
@@ -5368,22 +5390,22 @@
       <c r="C28" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
     </row>
     <row r="29" spans="2:17">
       <c r="B29" s="8" t="s">
@@ -5392,22 +5414,22 @@
       <c r="C29" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
     </row>
     <row r="30" spans="2:17">
       <c r="B30" s="8" t="s">
@@ -5416,22 +5438,22 @@
       <c r="C30" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10"/>
-      <c r="P30" s="10"/>
-      <c r="Q30" s="10"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
     </row>
     <row r="31" spans="2:17">
       <c r="B31" s="8" t="s">
@@ -5440,22 +5462,22 @@
       <c r="C31" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
     </row>
     <row r="32" spans="2:17">
       <c r="B32" s="8" t="s">
@@ -5464,32 +5486,37 @@
       <c r="C32" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D30:Q30"/>
-    <mergeCell ref="D31:Q31"/>
-    <mergeCell ref="D32:Q32"/>
-    <mergeCell ref="D24:Q24"/>
-    <mergeCell ref="D25:Q25"/>
-    <mergeCell ref="D26:Q26"/>
-    <mergeCell ref="D27:Q27"/>
-    <mergeCell ref="D28:Q28"/>
-    <mergeCell ref="D29:Q29"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="D13:Q13"/>
+    <mergeCell ref="D4:Q4"/>
+    <mergeCell ref="D5:Q5"/>
+    <mergeCell ref="D6:Q6"/>
+    <mergeCell ref="D7:Q7"/>
+    <mergeCell ref="D8:Q8"/>
+    <mergeCell ref="D9:Q9"/>
+    <mergeCell ref="D10:Q10"/>
     <mergeCell ref="D23:Q23"/>
     <mergeCell ref="D3:Q3"/>
     <mergeCell ref="D11:Q11"/>
@@ -5503,15 +5530,15 @@
     <mergeCell ref="D20:Q20"/>
     <mergeCell ref="D21:Q21"/>
     <mergeCell ref="D22:Q22"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="D13:Q13"/>
-    <mergeCell ref="D4:Q4"/>
-    <mergeCell ref="D5:Q5"/>
-    <mergeCell ref="D6:Q6"/>
-    <mergeCell ref="D7:Q7"/>
-    <mergeCell ref="D8:Q8"/>
-    <mergeCell ref="D9:Q9"/>
-    <mergeCell ref="D10:Q10"/>
+    <mergeCell ref="D30:Q30"/>
+    <mergeCell ref="D31:Q31"/>
+    <mergeCell ref="D32:Q32"/>
+    <mergeCell ref="D24:Q24"/>
+    <mergeCell ref="D25:Q25"/>
+    <mergeCell ref="D26:Q26"/>
+    <mergeCell ref="D27:Q27"/>
+    <mergeCell ref="D28:Q28"/>
+    <mergeCell ref="D29:Q29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajust data to ANLA, Colecciones and I2D datasets
</commit_message>
<xml_diff>
--- a/addicional_data/Indicaciones-Mapeos_2023.xlsx
+++ b/addicional_data/Indicaciones-Mapeos_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Cristian_data\Humboldt\Git\Unif_biological_data_-set16-\addicional_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3B4D65-B857-40D0-9A1B-146F1FE6EA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E43756-1757-4221-992B-C9BEB884C2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="774" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="774" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="blank2keep" sheetId="1" r:id="rId1"/>
@@ -18,26 +18,14 @@
     <sheet name="camposSet16" sheetId="4" r:id="rId3"/>
     <sheet name="oficial_data" sheetId="12" r:id="rId4"/>
     <sheet name="Definitions" sheetId="15" r:id="rId5"/>
+    <sheet name="Hoja1" sheetId="16" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="447">
   <si>
     <t>lon</t>
   </si>
@@ -159,9 +147,6 @@
     <t>coordinateUncertaintyInMeters</t>
   </si>
   <si>
-    <t>geodeticDatum</t>
-  </si>
-  <si>
     <t>decimalLongitude</t>
   </si>
   <si>
@@ -171,12 +156,6 @@
     <t>verbatimCoordinateSystem</t>
   </si>
   <si>
-    <t>verbatimLongitude</t>
-  </si>
-  <si>
-    <t>verbatimLatitude</t>
-  </si>
-  <si>
     <t>maximumElevationInMeters</t>
   </si>
   <si>
@@ -1270,9 +1249,6 @@
   </si>
   <si>
     <t>ANLA_dep</t>
-  </si>
-  <si>
-    <t>origen</t>
   </si>
   <si>
     <t>COUNTRY CODE</t>
@@ -1388,6 +1364,9 @@
   </si>
   <si>
     <t>The name of the first or species epithet of the scientificName.</t>
+  </si>
+  <si>
+    <t>Numero.de.Inventario</t>
   </si>
 </sst>
 </file>
@@ -2278,11 +2257,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:IE14"/>
+  <dimension ref="A1:ID14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ13" sqref="AJ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15"/>
@@ -2290,140 +2269,140 @@
     <col min="7" max="7" width="113.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:239">
+    <row r="1" spans="1:238">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="M1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="O1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="P1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="R1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="S1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="T1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="U1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="V1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="W1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="X1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="Y1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Z1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="AA1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AB1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="AC1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AD1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="AE1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AF1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AG1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AH1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="AI1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="AJ1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="AK1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AL1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AM1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AN1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="AO1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AP1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AQ1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:239">
+    <row r="2" spans="1:238">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -2438,42 +2417,42 @@
         <v>15</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="T2" t="s">
         <v>5</v>
       </c>
       <c r="W2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="X2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:239">
+    <row r="3" spans="1:238">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -2501,66 +2480,66 @@
         <v>20</v>
       </c>
       <c r="Y3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Z3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="AA3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AB3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AF3" t="s">
         <v>15</v>
       </c>
       <c r="AG3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AH3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AI3" t="s">
         <v>5</v>
       </c>
       <c r="AJ3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK3" t="s">
         <v>41</v>
       </c>
-      <c r="AK3" t="s">
-        <v>42</v>
-      </c>
       <c r="AN3" s="8" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="AP3" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:239">
+    <row r="4" spans="1:238">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I4" t="s">
         <v>26</v>
@@ -2569,7 +2548,7 @@
         <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M4" t="s">
         <v>22</v>
@@ -2581,120 +2560,120 @@
         <v>8</v>
       </c>
       <c r="P4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="R4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="S4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="T4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="U4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="V4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="W4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="X4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Y4" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="Z4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="AA4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AB4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="AC4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="AD4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AE4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AF4" t="s">
         <v>15</v>
       </c>
       <c r="AG4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AH4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AI4" t="s">
         <v>5</v>
       </c>
       <c r="AJ4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AK4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AL4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AM4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AN4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AO4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AP4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AQ4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AR4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="AS4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="AT4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AU4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="AV4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AW4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AX4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AY4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="AZ4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:239">
+    <row r="5" spans="1:238">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -2702,15 +2681,13 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>110</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="AP5" s="2"/>
       <c r="BJ5" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="BK5" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="BN5" s="2" t="s">
         <v>11</v>
@@ -2719,511 +2696,508 @@
         <v>16</v>
       </c>
       <c r="BS5" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="BU5" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="CW5" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="DA5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="DB5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="DC5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="DO5" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="DS5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="DT5" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="DV5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="DW5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="EE5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="EF5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="EG5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="EH5" s="2"/>
-      <c r="GC5" t="s">
+      <c r="GE5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="GF5" s="2" t="s">
-        <v>27</v>
+      <c r="GJ5" t="s">
+        <v>26</v>
       </c>
       <c r="GK5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="GL5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="GM5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="GN5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="GO5" t="s">
-        <v>22</v>
-      </c>
-      <c r="GP5" t="s">
         <v>21</v>
       </c>
-      <c r="GR5" t="s">
+      <c r="GQ5" t="s">
         <v>20</v>
       </c>
-      <c r="HD5" s="2" t="s">
-        <v>103</v>
+      <c r="HC5" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:239">
+    <row r="6" spans="1:238">
       <c r="A6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" t="s">
+        <v>253</v>
+      </c>
+      <c r="F6" t="s">
         <v>254</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>255</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>256</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
         <v>257</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>258</v>
       </c>
-      <c r="H6" t="s">
+      <c r="K6" t="s">
         <v>259</v>
       </c>
-      <c r="I6" t="s">
+      <c r="L6" t="s">
+        <v>105</v>
+      </c>
+      <c r="M6" t="s">
         <v>260</v>
       </c>
-      <c r="J6" t="s">
+      <c r="N6" t="s">
         <v>261</v>
       </c>
-      <c r="K6" t="s">
+      <c r="O6" t="s">
         <v>262</v>
       </c>
-      <c r="L6" t="s">
+      <c r="P6" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6" t="s">
+        <v>104</v>
+      </c>
+      <c r="S6" t="s">
+        <v>263</v>
+      </c>
+      <c r="T6" t="s">
+        <v>264</v>
+      </c>
+      <c r="U6" t="s">
+        <v>265</v>
+      </c>
+      <c r="V6" t="s">
+        <v>94</v>
+      </c>
+      <c r="W6" t="s">
+        <v>266</v>
+      </c>
+      <c r="X6" t="s">
+        <v>267</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>268</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>269</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>270</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>272</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>273</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>274</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>275</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>276</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>277</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>278</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>279</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>280</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>281</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>282</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>283</v>
+      </c>
+      <c r="AS6" t="s">
         <v>108</v>
       </c>
-      <c r="M6" t="s">
-        <v>263</v>
-      </c>
-      <c r="N6" t="s">
-        <v>264</v>
-      </c>
-      <c r="O6" t="s">
-        <v>265</v>
-      </c>
-      <c r="P6" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>77</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="AT6" t="s">
+        <v>284</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>285</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>286</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>103</v>
+      </c>
+      <c r="AY6" t="s">
         <v>107</v>
       </c>
-      <c r="S6" t="s">
-        <v>266</v>
-      </c>
-      <c r="T6" t="s">
-        <v>267</v>
-      </c>
-      <c r="U6" t="s">
-        <v>268</v>
-      </c>
-      <c r="V6" t="s">
-        <v>97</v>
-      </c>
-      <c r="W6" t="s">
-        <v>269</v>
-      </c>
-      <c r="X6" t="s">
-        <v>270</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>271</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>272</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>274</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>275</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>276</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>277</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>278</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>279</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>280</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL6" t="s">
+      <c r="AZ6" t="s">
+        <v>287</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>288</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>289</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>290</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>106</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>95</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>291</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>62</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>118</v>
+      </c>
+      <c r="BJ6" t="s">
         <v>67</v>
       </c>
-      <c r="AM6" t="s">
-        <v>282</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>283</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>284</v>
-      </c>
-      <c r="AP6" t="s">
+      <c r="BK6" t="s">
+        <v>66</v>
+      </c>
+      <c r="BL6" t="s">
         <v>117</v>
       </c>
-      <c r="AQ6" t="s">
-        <v>285</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>286</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>287</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>288</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>289</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>106</v>
-      </c>
-      <c r="AY6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>290</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>291</v>
-      </c>
-      <c r="BB6" t="s">
-        <v>292</v>
-      </c>
-      <c r="BC6" t="s">
-        <v>293</v>
-      </c>
-      <c r="BD6" t="s">
-        <v>109</v>
-      </c>
-      <c r="BE6" t="s">
-        <v>98</v>
-      </c>
-      <c r="BF6" t="s">
-        <v>294</v>
-      </c>
-      <c r="BG6" t="s">
-        <v>66</v>
-      </c>
-      <c r="BH6" t="s">
-        <v>65</v>
-      </c>
-      <c r="BI6" t="s">
-        <v>121</v>
-      </c>
-      <c r="BJ6" t="s">
-        <v>70</v>
-      </c>
-      <c r="BK6" t="s">
-        <v>69</v>
-      </c>
-      <c r="BL6" t="s">
-        <v>120</v>
-      </c>
       <c r="BM6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="BN6" t="s">
         <v>11</v>
       </c>
       <c r="BO6" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="BP6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BQ6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="BR6" t="s">
         <v>16</v>
       </c>
       <c r="BS6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="BT6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="BU6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="BV6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="BW6" t="s">
+        <v>294</v>
+      </c>
+      <c r="BX6" t="s">
+        <v>295</v>
+      </c>
+      <c r="BY6" t="s">
+        <v>85</v>
+      </c>
+      <c r="BZ6" t="s">
+        <v>86</v>
+      </c>
+      <c r="CA6" t="s">
+        <v>58</v>
+      </c>
+      <c r="CB6" t="s">
+        <v>119</v>
+      </c>
+      <c r="CC6" t="s">
+        <v>72</v>
+      </c>
+      <c r="CD6" t="s">
+        <v>57</v>
+      </c>
+      <c r="CE6" t="s">
+        <v>89</v>
+      </c>
+      <c r="CF6" t="s">
+        <v>56</v>
+      </c>
+      <c r="CG6" t="s">
+        <v>53</v>
+      </c>
+      <c r="CH6" t="s">
+        <v>121</v>
+      </c>
+      <c r="CI6" t="s">
+        <v>120</v>
+      </c>
+      <c r="CJ6" t="s">
+        <v>55</v>
+      </c>
+      <c r="CK6" t="s">
+        <v>61</v>
+      </c>
+      <c r="CL6" t="s">
+        <v>296</v>
+      </c>
+      <c r="CM6" t="s">
         <v>297</v>
       </c>
-      <c r="BX6" t="s">
+      <c r="CN6" t="s">
         <v>298</v>
       </c>
-      <c r="BY6" t="s">
+      <c r="CO6" t="s">
+        <v>122</v>
+      </c>
+      <c r="CP6" t="s">
+        <v>299</v>
+      </c>
+      <c r="CQ6" t="s">
+        <v>54</v>
+      </c>
+      <c r="CR6" t="s">
+        <v>300</v>
+      </c>
+      <c r="CS6" t="s">
+        <v>301</v>
+      </c>
+      <c r="CT6" t="s">
+        <v>77</v>
+      </c>
+      <c r="CU6" t="s">
+        <v>302</v>
+      </c>
+      <c r="CV6" t="s">
+        <v>303</v>
+      </c>
+      <c r="CW6" t="s">
+        <v>52</v>
+      </c>
+      <c r="CX6" t="s">
         <v>88</v>
       </c>
-      <c r="BZ6" t="s">
-        <v>89</v>
-      </c>
-      <c r="CA6" t="s">
-        <v>61</v>
-      </c>
-      <c r="CB6" t="s">
-        <v>122</v>
-      </c>
-      <c r="CC6" t="s">
-        <v>75</v>
-      </c>
-      <c r="CD6" t="s">
-        <v>60</v>
-      </c>
-      <c r="CE6" t="s">
-        <v>92</v>
-      </c>
-      <c r="CF6" t="s">
-        <v>59</v>
-      </c>
-      <c r="CG6" t="s">
-        <v>56</v>
-      </c>
-      <c r="CH6" t="s">
-        <v>124</v>
-      </c>
-      <c r="CI6" t="s">
-        <v>123</v>
-      </c>
-      <c r="CJ6" t="s">
-        <v>58</v>
-      </c>
-      <c r="CK6" t="s">
-        <v>64</v>
-      </c>
-      <c r="CL6" t="s">
-        <v>299</v>
-      </c>
-      <c r="CM6" t="s">
-        <v>300</v>
-      </c>
-      <c r="CN6" t="s">
-        <v>301</v>
-      </c>
-      <c r="CO6" t="s">
-        <v>125</v>
-      </c>
-      <c r="CP6" t="s">
-        <v>302</v>
-      </c>
-      <c r="CQ6" t="s">
-        <v>57</v>
-      </c>
-      <c r="CR6" t="s">
-        <v>303</v>
-      </c>
-      <c r="CS6" t="s">
+      <c r="CY6" t="s">
         <v>304</v>
       </c>
-      <c r="CT6" t="s">
+      <c r="CZ6" t="s">
+        <v>305</v>
+      </c>
+      <c r="DA6" t="s">
+        <v>78</v>
+      </c>
+      <c r="DB6" t="s">
+        <v>79</v>
+      </c>
+      <c r="DC6" t="s">
         <v>80</v>
       </c>
-      <c r="CU6" t="s">
-        <v>305</v>
-      </c>
-      <c r="CV6" t="s">
+      <c r="DD6" t="s">
+        <v>110</v>
+      </c>
+      <c r="DE6" t="s">
+        <v>50</v>
+      </c>
+      <c r="DF6" t="s">
+        <v>84</v>
+      </c>
+      <c r="DG6" t="s">
+        <v>83</v>
+      </c>
+      <c r="DH6" t="s">
         <v>306</v>
       </c>
-      <c r="CW6" t="s">
-        <v>55</v>
-      </c>
-      <c r="CX6" t="s">
-        <v>91</v>
-      </c>
-      <c r="CY6" t="s">
+      <c r="DI6" t="s">
         <v>307</v>
       </c>
-      <c r="CZ6" t="s">
+      <c r="DJ6" t="s">
         <v>308</v>
       </c>
-      <c r="DA6" t="s">
+      <c r="DK6" t="s">
+        <v>51</v>
+      </c>
+      <c r="DL6" t="s">
+        <v>99</v>
+      </c>
+      <c r="DM6" t="s">
+        <v>309</v>
+      </c>
+      <c r="DN6" t="s">
+        <v>310</v>
+      </c>
+      <c r="DO6" t="s">
+        <v>49</v>
+      </c>
+      <c r="DP6" t="s">
         <v>81</v>
       </c>
-      <c r="DB6" t="s">
-        <v>82</v>
-      </c>
-      <c r="DC6" t="s">
-        <v>83</v>
-      </c>
-      <c r="DD6" t="s">
-        <v>113</v>
-      </c>
-      <c r="DE6" t="s">
-        <v>53</v>
-      </c>
-      <c r="DF6" t="s">
-        <v>87</v>
-      </c>
-      <c r="DG6" t="s">
-        <v>86</v>
-      </c>
-      <c r="DH6" t="s">
-        <v>309</v>
-      </c>
-      <c r="DI6" t="s">
-        <v>310</v>
-      </c>
-      <c r="DJ6" t="s">
+      <c r="DQ6" t="s">
         <v>311</v>
       </c>
-      <c r="DK6" t="s">
-        <v>54</v>
-      </c>
-      <c r="DL6" t="s">
-        <v>102</v>
-      </c>
-      <c r="DM6" t="s">
-        <v>312</v>
-      </c>
-      <c r="DN6" t="s">
-        <v>313</v>
-      </c>
-      <c r="DO6" t="s">
-        <v>52</v>
-      </c>
-      <c r="DP6" t="s">
-        <v>84</v>
-      </c>
-      <c r="DQ6" t="s">
-        <v>314</v>
-      </c>
       <c r="DR6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="DS6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="DT6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="DU6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="DV6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="DW6" t="s">
         <v>5</v>
       </c>
       <c r="DX6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="DY6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="DZ6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="EA6" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="EB6" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="EC6" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="ED6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="EE6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="EF6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="EG6" t="s">
         <v>39</v>
       </c>
       <c r="EH6" t="s">
+        <v>315</v>
+      </c>
+      <c r="EI6" t="s">
+        <v>316</v>
+      </c>
+      <c r="EJ6" t="s">
+        <v>42</v>
+      </c>
+      <c r="EK6" t="s">
+        <v>70</v>
+      </c>
+      <c r="EL6" t="s">
+        <v>116</v>
+      </c>
+      <c r="EM6" t="s">
+        <v>317</v>
+      </c>
+      <c r="EN6" t="s">
         <v>318</v>
-      </c>
-      <c r="EI6" t="s">
-        <v>319</v>
-      </c>
-      <c r="EJ6" t="s">
-        <v>43</v>
-      </c>
-      <c r="EK6" t="s">
-        <v>73</v>
-      </c>
-      <c r="EL6" t="s">
-        <v>119</v>
-      </c>
-      <c r="EM6" t="s">
-        <v>320</v>
-      </c>
-      <c r="EN6" t="s">
-        <v>321</v>
       </c>
       <c r="EO6" t="s">
         <v>38</v>
@@ -3238,67 +3212,67 @@
         <v>35</v>
       </c>
       <c r="ES6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="ET6" t="s">
         <v>34</v>
       </c>
       <c r="EU6" t="s">
+        <v>319</v>
+      </c>
+      <c r="EV6" t="s">
+        <v>320</v>
+      </c>
+      <c r="EW6" t="s">
+        <v>321</v>
+      </c>
+      <c r="EX6" t="s">
         <v>322</v>
       </c>
-      <c r="EV6" t="s">
+      <c r="EY6" t="s">
         <v>323</v>
       </c>
-      <c r="EW6" t="s">
+      <c r="EZ6" t="s">
         <v>324</v>
       </c>
-      <c r="EX6" t="s">
+      <c r="FA6" t="s">
         <v>325</v>
       </c>
-      <c r="EY6" t="s">
+      <c r="FB6" t="s">
         <v>326</v>
       </c>
-      <c r="EZ6" t="s">
+      <c r="FC6" t="s">
         <v>327</v>
       </c>
-      <c r="FA6" t="s">
+      <c r="FD6" t="s">
         <v>328</v>
       </c>
-      <c r="FB6" t="s">
+      <c r="FE6" t="s">
         <v>329</v>
       </c>
-      <c r="FC6" t="s">
+      <c r="FF6" t="s">
         <v>330</v>
       </c>
-      <c r="FD6" t="s">
+      <c r="FG6" t="s">
         <v>331</v>
       </c>
-      <c r="FE6" t="s">
+      <c r="FH6" t="s">
         <v>332</v>
       </c>
-      <c r="FF6" t="s">
+      <c r="FI6" t="s">
+        <v>210</v>
+      </c>
+      <c r="FJ6" t="s">
+        <v>209</v>
+      </c>
+      <c r="FK6" t="s">
+        <v>208</v>
+      </c>
+      <c r="FL6" t="s">
+        <v>207</v>
+      </c>
+      <c r="FM6" t="s">
         <v>333</v>
-      </c>
-      <c r="FG6" t="s">
-        <v>334</v>
-      </c>
-      <c r="FH6" t="s">
-        <v>335</v>
-      </c>
-      <c r="FI6" t="s">
-        <v>213</v>
-      </c>
-      <c r="FJ6" t="s">
-        <v>212</v>
-      </c>
-      <c r="FK6" t="s">
-        <v>211</v>
-      </c>
-      <c r="FL6" t="s">
-        <v>210</v>
-      </c>
-      <c r="FM6" t="s">
-        <v>336</v>
       </c>
       <c r="FN6" t="s">
         <v>29</v>
@@ -3316,365 +3290,410 @@
         <v>31</v>
       </c>
       <c r="FS6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="FT6" t="s">
         <v>30</v>
       </c>
       <c r="FU6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="FV6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="FW6" t="s">
+        <v>335</v>
+      </c>
+      <c r="FX6" t="s">
+        <v>336</v>
+      </c>
+      <c r="FY6" t="s">
+        <v>337</v>
+      </c>
+      <c r="FZ6" t="s">
         <v>338</v>
       </c>
-      <c r="FX6" t="s">
+      <c r="GA6" t="s">
         <v>339</v>
       </c>
-      <c r="FY6" t="s">
+      <c r="GB6" t="s">
         <v>340</v>
       </c>
-      <c r="FZ6" t="s">
+      <c r="GC6" t="s">
+        <v>91</v>
+      </c>
+      <c r="GD6" t="s">
         <v>341</v>
       </c>
-      <c r="GA6" t="s">
+      <c r="GE6" t="s">
+        <v>27</v>
+      </c>
+      <c r="GF6" t="s">
+        <v>90</v>
+      </c>
+      <c r="GG6" t="s">
         <v>342</v>
       </c>
-      <c r="GB6" t="s">
+      <c r="GH6" t="s">
         <v>343</v>
       </c>
-      <c r="GC6" t="s">
-        <v>27</v>
-      </c>
-      <c r="GD6" t="s">
-        <v>94</v>
-      </c>
-      <c r="GE6" t="s">
+      <c r="GI6" t="s">
+        <v>115</v>
+      </c>
+      <c r="GJ6" t="s">
+        <v>26</v>
+      </c>
+      <c r="GK6" t="s">
+        <v>25</v>
+      </c>
+      <c r="GL6" t="s">
+        <v>24</v>
+      </c>
+      <c r="GM6" t="s">
+        <v>23</v>
+      </c>
+      <c r="GN6" t="s">
+        <v>22</v>
+      </c>
+      <c r="GO6" t="s">
+        <v>21</v>
+      </c>
+      <c r="GP6" t="s">
+        <v>206</v>
+      </c>
+      <c r="GQ6" t="s">
+        <v>20</v>
+      </c>
+      <c r="GR6" t="s">
+        <v>97</v>
+      </c>
+      <c r="GS6" t="s">
+        <v>19</v>
+      </c>
+      <c r="GT6" t="s">
+        <v>96</v>
+      </c>
+      <c r="GU6" t="s">
+        <v>18</v>
+      </c>
+      <c r="GV6" t="s">
+        <v>113</v>
+      </c>
+      <c r="GW6" t="s">
+        <v>92</v>
+      </c>
+      <c r="GX6" t="s">
         <v>344</v>
       </c>
-      <c r="GF6" t="s">
-        <v>27</v>
-      </c>
-      <c r="GG6" t="s">
+      <c r="GY6" t="s">
         <v>93</v>
       </c>
-      <c r="GH6" t="s">
+      <c r="GZ6" t="s">
         <v>345</v>
       </c>
-      <c r="GI6" t="s">
+      <c r="HA6" t="s">
         <v>346</v>
       </c>
-      <c r="GJ6" t="s">
-        <v>118</v>
-      </c>
-      <c r="GK6" t="s">
-        <v>26</v>
-      </c>
-      <c r="GL6" t="s">
-        <v>25</v>
-      </c>
-      <c r="GM6" t="s">
-        <v>24</v>
-      </c>
-      <c r="GN6" t="s">
-        <v>23</v>
-      </c>
-      <c r="GO6" t="s">
-        <v>22</v>
-      </c>
-      <c r="GP6" t="s">
-        <v>21</v>
-      </c>
-      <c r="GQ6" t="s">
-        <v>209</v>
-      </c>
-      <c r="GR6" t="s">
-        <v>20</v>
-      </c>
-      <c r="GS6" t="s">
-        <v>100</v>
-      </c>
-      <c r="GT6" t="s">
-        <v>19</v>
-      </c>
-      <c r="GU6" t="s">
-        <v>99</v>
-      </c>
-      <c r="GV6" t="s">
-        <v>18</v>
-      </c>
-      <c r="GW6" t="s">
-        <v>116</v>
-      </c>
-      <c r="GX6" t="s">
-        <v>95</v>
-      </c>
-      <c r="GY6" t="s">
+      <c r="HB6" t="s">
         <v>347</v>
       </c>
-      <c r="GZ6" t="s">
-        <v>96</v>
-      </c>
-      <c r="HA6" t="s">
+      <c r="HC6" t="s">
         <v>348</v>
       </c>
-      <c r="HB6" t="s">
+      <c r="HD6" t="s">
         <v>349</v>
       </c>
-      <c r="HC6" t="s">
+      <c r="HE6" t="s">
         <v>350</v>
       </c>
-      <c r="HD6" t="s">
+      <c r="HF6" t="s">
         <v>351</v>
       </c>
-      <c r="HE6" t="s">
+      <c r="HG6" t="s">
         <v>352</v>
       </c>
-      <c r="HF6" t="s">
+      <c r="HH6" t="s">
         <v>353</v>
       </c>
-      <c r="HG6" t="s">
+      <c r="HI6" t="s">
         <v>354</v>
       </c>
-      <c r="HH6" t="s">
+      <c r="HJ6" t="s">
         <v>355</v>
       </c>
-      <c r="HI6" t="s">
+      <c r="HK6" t="s">
         <v>356</v>
       </c>
-      <c r="HJ6" t="s">
+      <c r="HL6" t="s">
         <v>357</v>
       </c>
-      <c r="HK6" t="s">
+      <c r="HM6" t="s">
         <v>358</v>
       </c>
-      <c r="HL6" t="s">
+      <c r="HN6" t="s">
         <v>359</v>
       </c>
-      <c r="HM6" t="s">
+      <c r="HO6" t="s">
         <v>360</v>
       </c>
-      <c r="HN6" t="s">
+      <c r="HP6" t="s">
         <v>361</v>
       </c>
-      <c r="HO6" t="s">
+      <c r="HQ6" t="s">
         <v>362</v>
       </c>
-      <c r="HP6" t="s">
+      <c r="HR6" t="s">
         <v>363</v>
       </c>
-      <c r="HQ6" t="s">
+      <c r="HS6" t="s">
         <v>364</v>
       </c>
-      <c r="HR6" t="s">
+      <c r="HT6" t="s">
         <v>365</v>
       </c>
-      <c r="HS6" t="s">
+      <c r="HU6" t="s">
         <v>366</v>
       </c>
-      <c r="HT6" t="s">
+      <c r="HV6" t="s">
         <v>367</v>
       </c>
-      <c r="HU6" t="s">
+      <c r="HW6" t="s">
+        <v>8</v>
+      </c>
+      <c r="HX6" t="s">
         <v>368</v>
       </c>
-      <c r="HV6" t="s">
+      <c r="HY6" t="s">
         <v>369</v>
       </c>
-      <c r="HW6" t="s">
+      <c r="HZ6" t="s">
         <v>370</v>
       </c>
-      <c r="HX6" t="s">
-        <v>8</v>
-      </c>
-      <c r="HY6" t="s">
+      <c r="IA6" t="s">
         <v>371</v>
       </c>
-      <c r="HZ6" t="s">
+      <c r="IB6" t="s">
         <v>372</v>
       </c>
-      <c r="IA6" t="s">
+      <c r="IC6" t="s">
         <v>373</v>
       </c>
-      <c r="IB6" t="s">
+      <c r="ID6" t="s">
         <v>374</v>
       </c>
-      <c r="IC6" t="s">
-        <v>375</v>
-      </c>
-      <c r="ID6" t="s">
-        <v>376</v>
-      </c>
-      <c r="IE6" t="s">
-        <v>377</v>
-      </c>
     </row>
-    <row r="7" spans="1:239">
+    <row r="7" spans="1:238">
       <c r="A7" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7" t="s">
+        <v>15</v>
+      </c>
+      <c r="S7" t="s">
+        <v>45</v>
+      </c>
+      <c r="U7" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" t="s">
+        <v>67</v>
+      </c>
+      <c r="W7" t="s">
+        <v>66</v>
+      </c>
+      <c r="X7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" t="s">
-        <v>48</v>
-      </c>
-      <c r="M7" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" t="s">
-        <v>70</v>
-      </c>
-      <c r="O7" t="s">
-        <v>69</v>
-      </c>
-      <c r="P7" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>68</v>
-      </c>
-      <c r="R7" t="s">
-        <v>62</v>
-      </c>
-      <c r="S7" t="s">
-        <v>55</v>
-      </c>
-      <c r="T7" t="s">
+      <c r="AB7" t="s">
         <v>39</v>
       </c>
-      <c r="U7" t="s">
-        <v>103</v>
-      </c>
-      <c r="V7" t="s">
-        <v>406</v>
+      <c r="AC7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>403</v>
       </c>
     </row>
-    <row r="8" spans="1:239">
+    <row r="8" spans="1:238">
       <c r="A8" t="s">
-        <v>404</v>
-      </c>
-      <c r="B8" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>446</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
         <v>47</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
         <v>5</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>27</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" t="s">
         <v>15</v>
       </c>
-      <c r="K8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="S8" t="s">
         <v>46</v>
       </c>
-      <c r="M8" t="s">
-        <v>41</v>
-      </c>
-      <c r="N8" t="s">
-        <v>70</v>
-      </c>
-      <c r="O8" t="s">
-        <v>69</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="T8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U8" t="s">
+        <v>40</v>
+      </c>
+      <c r="V8" t="s">
+        <v>67</v>
+      </c>
+      <c r="W8" t="s">
+        <v>66</v>
+      </c>
+      <c r="X8" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" t="s">
-        <v>68</v>
-      </c>
-      <c r="R8" t="s">
-        <v>62</v>
-      </c>
-      <c r="S8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="Y8" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB8" t="s">
         <v>39</v>
       </c>
-      <c r="U8" t="s">
-        <v>47</v>
-      </c>
-      <c r="V8" t="s">
-        <v>405</v>
+      <c r="AC8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>402</v>
       </c>
     </row>
-    <row r="9" spans="1:239">
+    <row r="9" spans="1:238">
       <c r="A9" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" t="s">
         <v>16</v>
       </c>
       <c r="N9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="R9" t="s">
+        <v>40</v>
+      </c>
+      <c r="S9" t="s">
         <v>41</v>
-      </c>
-      <c r="S9" t="s">
-        <v>42</v>
       </c>
       <c r="U9" t="s">
         <v>25</v>
@@ -3695,113 +3714,113 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:239">
+    <row r="10" spans="1:238">
       <c r="A10" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>383</v>
+      </c>
+      <c r="D10" t="s">
+        <v>388</v>
+      </c>
+      <c r="E10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F10" t="s">
+        <v>389</v>
+      </c>
+      <c r="G10" t="s">
+        <v>390</v>
+      </c>
+      <c r="H10" t="s">
+        <v>376</v>
+      </c>
+      <c r="I10" t="s">
+        <v>391</v>
+      </c>
+      <c r="J10" t="s">
+        <v>392</v>
+      </c>
+      <c r="K10" t="s">
+        <v>393</v>
+      </c>
+      <c r="L10" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" t="s">
+        <v>394</v>
+      </c>
+      <c r="N10" t="s">
+        <v>395</v>
+      </c>
+      <c r="O10" t="s">
+        <v>396</v>
+      </c>
+      <c r="P10" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>398</v>
+      </c>
+      <c r="R10" t="s">
+        <v>399</v>
+      </c>
+      <c r="S10" t="s">
+        <v>400</v>
+      </c>
+      <c r="T10" t="s">
+        <v>382</v>
+      </c>
+      <c r="U10" t="s">
+        <v>377</v>
+      </c>
+      <c r="V10" t="s">
+        <v>215</v>
+      </c>
+      <c r="W10" t="s">
+        <v>214</v>
+      </c>
+      <c r="X10" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>212</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>378</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>379</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>380</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>384</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>385</v>
+      </c>
+      <c r="AE10" t="s">
         <v>386</v>
       </c>
-      <c r="D10" t="s">
-        <v>391</v>
-      </c>
-      <c r="E10" t="s">
-        <v>208</v>
-      </c>
-      <c r="F10" t="s">
-        <v>392</v>
-      </c>
-      <c r="G10" t="s">
-        <v>393</v>
-      </c>
-      <c r="H10" t="s">
-        <v>379</v>
-      </c>
-      <c r="I10" t="s">
-        <v>394</v>
-      </c>
-      <c r="J10" t="s">
-        <v>395</v>
-      </c>
-      <c r="K10" t="s">
-        <v>396</v>
-      </c>
-      <c r="L10" t="s">
-        <v>53</v>
-      </c>
-      <c r="M10" t="s">
-        <v>397</v>
-      </c>
-      <c r="N10" t="s">
-        <v>398</v>
-      </c>
-      <c r="O10" t="s">
-        <v>399</v>
-      </c>
-      <c r="P10" t="s">
-        <v>400</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>401</v>
-      </c>
-      <c r="R10" t="s">
-        <v>402</v>
-      </c>
-      <c r="S10" t="s">
-        <v>403</v>
-      </c>
-      <c r="T10" t="s">
-        <v>385</v>
-      </c>
-      <c r="U10" t="s">
-        <v>380</v>
-      </c>
-      <c r="V10" t="s">
-        <v>218</v>
-      </c>
-      <c r="W10" t="s">
-        <v>217</v>
-      </c>
-      <c r="X10" t="s">
-        <v>216</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>215</v>
-      </c>
-      <c r="Z10" t="s">
+      <c r="AF10" t="s">
+        <v>387</v>
+      </c>
+      <c r="AG10" t="s">
         <v>381</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AH10" t="s">
         <v>382</v>
       </c>
-      <c r="AB10" t="s">
-        <v>383</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>387</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>388</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>389</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>390</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>384</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>385</v>
-      </c>
     </row>
-    <row r="11" spans="1:239">
+    <row r="11" spans="1:238">
       <c r="A11" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -3810,43 +3829,43 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
         <v>5</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N11" t="s">
         <v>11</v>
       </c>
       <c r="O11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q11" t="s">
         <v>27</v>
@@ -3873,54 +3892,54 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:239">
+    <row r="12" spans="1:238">
       <c r="A12" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H12" t="s">
         <v>5</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K12" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="L12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="N12" t="s">
         <v>11</v>
       </c>
       <c r="O12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q12" t="s">
         <v>27</v>
@@ -3947,186 +3966,140 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:239">
-      <c r="A13" t="s">
-        <v>410</v>
+    <row r="13" spans="1:238" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
+        <v>407</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N13" t="s">
-        <v>70</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="N13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>50</v>
-      </c>
-      <c r="R13" t="s">
-        <v>68</v>
-      </c>
-      <c r="V13" t="s">
-        <v>55</v>
-      </c>
-      <c r="X13" t="s">
-        <v>103</v>
-      </c>
-      <c r="AA13" t="s">
+      <c r="P13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AB13" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD13" t="s">
+      <c r="AB13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AE13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AI13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AJ13" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="14" spans="1:239">
-      <c r="A14" t="s">
-        <v>410</v>
+    <row r="14" spans="1:238" s="1" customFormat="1">
+      <c r="A14" s="1" t="s">
+        <v>407</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K14" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" t="s">
-        <v>297</v>
-      </c>
-      <c r="M14" t="s">
-        <v>64</v>
-      </c>
-      <c r="N14" t="s">
-        <v>70</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="N14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q14" t="s">
-        <v>50</v>
-      </c>
-      <c r="R14" t="s">
-        <v>305</v>
-      </c>
-      <c r="S14" t="s">
-        <v>87</v>
-      </c>
-      <c r="T14" t="s">
-        <v>53</v>
-      </c>
-      <c r="U14" t="s">
-        <v>86</v>
-      </c>
-      <c r="V14" t="s">
-        <v>55</v>
-      </c>
-      <c r="W14" t="s">
-        <v>84</v>
-      </c>
-      <c r="X14" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE14" t="s">
+      <c r="AD14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AF14" t="s">
-        <v>98</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>411</v>
-      </c>
-      <c r="AI14" t="s">
+      <c r="AI14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -4154,7 +4127,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>16</v>
@@ -4166,7 +4139,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>15</v>
@@ -4187,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>4</v>
@@ -4199,7 +4172,7 @@
         <v>13</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>11</v>
@@ -4211,19 +4184,19 @@
         <v>12</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="W1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="Y1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -4231,31 +4204,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C2">
         <v>768987190</v>
       </c>
       <c r="D2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K2">
         <v>12.2075</v>
@@ -4264,25 +4237,25 @@
         <v>-72.37</v>
       </c>
       <c r="M2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N2">
         <v>20</v>
       </c>
       <c r="O2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="P2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="Q2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="R2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="S2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="T2" s="3">
         <v>39665</v>
@@ -4299,31 +4272,31 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C3">
         <v>768987186</v>
       </c>
       <c r="D3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K3">
         <v>12.2075</v>
@@ -4332,25 +4305,25 @@
         <v>-72.37</v>
       </c>
       <c r="M3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N3">
         <v>20</v>
       </c>
       <c r="O3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="P3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="Q3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="R3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="S3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="T3" s="3">
         <v>39665</v>
@@ -4367,31 +4340,31 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C4">
         <v>768987185</v>
       </c>
       <c r="D4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" t="s">
         <v>241</v>
       </c>
-      <c r="E4" t="s">
-        <v>241</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>240</v>
       </c>
-      <c r="G4" t="s">
-        <v>226</v>
-      </c>
-      <c r="H4" t="s">
-        <v>244</v>
-      </c>
-      <c r="I4" t="s">
-        <v>243</v>
-      </c>
       <c r="J4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K4">
         <v>12.2075</v>
@@ -4400,25 +4373,25 @@
         <v>-72.37</v>
       </c>
       <c r="M4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N4">
         <v>20</v>
       </c>
       <c r="O4" t="s">
+        <v>236</v>
+      </c>
+      <c r="P4" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q4" t="s">
         <v>239</v>
       </c>
-      <c r="P4" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>242</v>
-      </c>
       <c r="R4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="S4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="T4" s="3">
         <v>39937</v>
@@ -4435,31 +4408,31 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C5">
         <v>768987187</v>
       </c>
       <c r="D5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H5" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K5">
         <v>12.2075</v>
@@ -4468,25 +4441,25 @@
         <v>-72.37</v>
       </c>
       <c r="M5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N5">
         <v>20</v>
       </c>
       <c r="O5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="P5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="Q5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="R5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="S5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="T5" s="3">
         <v>39665</v>
@@ -4503,31 +4476,31 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C6">
         <v>322435545</v>
       </c>
       <c r="D6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="J6" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K6">
         <v>12.13</v>
@@ -4536,25 +4509,25 @@
         <v>-72.17</v>
       </c>
       <c r="M6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="O6" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="Q6">
         <v>1875943</v>
       </c>
       <c r="R6" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="S6" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="T6" s="3">
         <v>32299</v>
@@ -4571,31 +4544,31 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C7">
         <v>319607241</v>
       </c>
       <c r="D7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K7">
         <v>12.25</v>
@@ -4604,25 +4577,25 @@
         <v>-72.5</v>
       </c>
       <c r="M7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="O7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="Q7">
         <v>3423039</v>
       </c>
       <c r="R7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="S7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="T7" s="3">
         <v>34304</v>
@@ -4661,7 +4634,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>16</v>
@@ -4673,7 +4646,7 @@
         <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>15</v>
@@ -4694,7 +4667,7 @@
         <v>0</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>4</v>
@@ -4706,7 +4679,7 @@
         <v>13</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>11</v>
@@ -4718,19 +4691,19 @@
         <v>12</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:25">
@@ -4738,7 +4711,7 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -4751,8 +4724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D3B1B9-00CF-4FB8-9D54-860845AB5DAC}">
   <dimension ref="B1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C26:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4764,13 +4737,13 @@
   <sheetData>
     <row r="1" spans="2:17">
       <c r="B1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="2:17" ht="29.25" customHeight="1">
@@ -4781,7 +4754,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -4802,10 +4775,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -4827,7 +4800,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -4849,7 +4822,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -4871,7 +4844,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -4893,7 +4866,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -4915,7 +4888,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -4937,7 +4910,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -4959,7 +4932,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -4977,13 +4950,13 @@
     </row>
     <row r="11" spans="2:17">
       <c r="B11" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -5007,7 +4980,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -5028,10 +5001,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -5052,10 +5025,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -5079,7 +5052,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -5100,10 +5073,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -5124,10 +5097,10 @@
         <v>0</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -5145,13 +5118,13 @@
     </row>
     <row r="18" spans="2:17" ht="27.75" customHeight="1">
       <c r="B18" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -5172,10 +5145,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -5196,10 +5169,10 @@
         <v>14</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -5220,10 +5193,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -5241,13 +5214,13 @@
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -5271,7 +5244,7 @@
         <v>11</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
@@ -5292,10 +5265,10 @@
         <v>3</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
@@ -5316,10 +5289,10 @@
         <v>12</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
@@ -5337,13 +5310,13 @@
     </row>
     <row r="26" spans="2:17">
       <c r="B26" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
@@ -5361,13 +5334,13 @@
     </row>
     <row r="27" spans="2:17">
       <c r="B27" s="8" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
@@ -5385,13 +5358,13 @@
     </row>
     <row r="28" spans="2:17">
       <c r="B28" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -5409,13 +5382,13 @@
     </row>
     <row r="29" spans="2:17">
       <c r="B29" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -5433,13 +5406,13 @@
     </row>
     <row r="30" spans="2:17">
       <c r="B30" s="8" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
@@ -5457,13 +5430,13 @@
     </row>
     <row r="31" spans="2:17">
       <c r="B31" s="8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
@@ -5481,10 +5454,10 @@
     </row>
     <row r="32" spans="2:17">
       <c r="B32" s="8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -5543,4 +5516,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47536D8E-5125-49C7-AC64-C4F179280600}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ajust colnames to data 2023
</commit_message>
<xml_diff>
--- a/addicional_data/Indicaciones-Mapeos_2023.xlsx
+++ b/addicional_data/Indicaciones-Mapeos_2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Cristian_data\Humboldt\Git\Unif_biological_data_-set16-\addicional_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E43756-1757-4221-992B-C9BEB884C2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90422AF-8B66-43BC-B990-6738BFE67902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="774" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="447">
   <si>
     <t>lon</t>
   </si>
@@ -1916,11 +1916,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2260,8 +2260,8 @@
   <dimension ref="A1:ID14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ13" sqref="AJ13"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15"/>
@@ -3824,9 +3824,6 @@
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>49</v>
@@ -4753,22 +4750,22 @@
       <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
     </row>
     <row r="3" spans="2:17">
       <c r="B3" s="8" t="s">
@@ -4777,176 +4774,176 @@
       <c r="C3" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>434</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
     </row>
     <row r="4" spans="2:17">
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="10" t="s">
         <v>438</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
     </row>
     <row r="5" spans="2:17">
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>439</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
     </row>
     <row r="6" spans="2:17">
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="2:17">
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="10" t="s">
         <v>441</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="2:17">
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="2:17">
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>443</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
     </row>
     <row r="10" spans="2:17">
       <c r="B10" s="8"/>
       <c r="C10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
     </row>
     <row r="11" spans="2:17">
       <c r="B11" s="8" t="s">
@@ -4955,22 +4952,22 @@
       <c r="C11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="2:17">
       <c r="B12" s="8" t="s">
@@ -4979,22 +4976,22 @@
       <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
     </row>
     <row r="13" spans="2:17">
       <c r="B13" s="8" t="s">
@@ -5003,22 +5000,22 @@
       <c r="C13" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
     </row>
     <row r="14" spans="2:17" ht="26.25" customHeight="1">
       <c r="B14" s="8" t="s">
@@ -5027,22 +5024,22 @@
       <c r="C14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
     </row>
     <row r="15" spans="2:17">
       <c r="B15" s="8" t="s">
@@ -5051,22 +5048,22 @@
       <c r="C15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
     </row>
     <row r="16" spans="2:17">
       <c r="B16" s="8" t="s">
@@ -5075,22 +5072,22 @@
       <c r="C16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="2:17">
       <c r="B17" s="8" t="s">
@@ -5099,22 +5096,22 @@
       <c r="C17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="2:17" ht="27.75" customHeight="1">
       <c r="B18" s="8" t="s">
@@ -5123,22 +5120,22 @@
       <c r="C18" s="8" t="s">
         <v>417</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
     </row>
     <row r="19" spans="2:17">
       <c r="B19" s="8" t="s">
@@ -5147,22 +5144,22 @@
       <c r="C19" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
     </row>
     <row r="20" spans="2:17">
       <c r="B20" s="8" t="s">
@@ -5171,22 +5168,22 @@
       <c r="C20" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
     </row>
     <row r="21" spans="2:17">
       <c r="B21" s="8" t="s">
@@ -5195,22 +5192,22 @@
       <c r="C21" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="10" t="s">
         <v>421</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="8" t="s">
@@ -5219,22 +5216,22 @@
       <c r="C22" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="10" t="s">
         <v>422</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
     </row>
     <row r="23" spans="2:17">
       <c r="B23" s="8" t="s">
@@ -5243,22 +5240,22 @@
       <c r="C23" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
     </row>
     <row r="24" spans="2:17" ht="27" customHeight="1">
       <c r="B24" s="8" t="s">
@@ -5267,22 +5264,22 @@
       <c r="C24" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
     </row>
     <row r="25" spans="2:17">
       <c r="B25" s="8" t="s">
@@ -5291,22 +5288,22 @@
       <c r="C25" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
     </row>
     <row r="26" spans="2:17">
       <c r="B26" s="8" t="s">
@@ -5315,22 +5312,22 @@
       <c r="C26" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="10" t="s">
         <v>426</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
     </row>
     <row r="27" spans="2:17">
       <c r="B27" s="8" t="s">
@@ -5339,22 +5336,22 @@
       <c r="C27" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
     </row>
     <row r="28" spans="2:17">
       <c r="B28" s="8" t="s">
@@ -5363,22 +5360,22 @@
       <c r="C28" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
     </row>
     <row r="29" spans="2:17">
       <c r="B29" s="8" t="s">
@@ -5387,22 +5384,22 @@
       <c r="C29" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
     </row>
     <row r="30" spans="2:17">
       <c r="B30" s="8" t="s">
@@ -5411,22 +5408,22 @@
       <c r="C30" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
     </row>
     <row r="31" spans="2:17">
       <c r="B31" s="8" t="s">
@@ -5435,22 +5432,22 @@
       <c r="C31" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
     </row>
     <row r="32" spans="2:17">
       <c r="B32" s="8" t="s">
@@ -5459,20 +5456,20 @@
       <c r="C32" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
@@ -5481,15 +5478,15 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="D13:Q13"/>
-    <mergeCell ref="D4:Q4"/>
-    <mergeCell ref="D5:Q5"/>
-    <mergeCell ref="D6:Q6"/>
-    <mergeCell ref="D7:Q7"/>
-    <mergeCell ref="D8:Q8"/>
-    <mergeCell ref="D9:Q9"/>
-    <mergeCell ref="D10:Q10"/>
+    <mergeCell ref="D30:Q30"/>
+    <mergeCell ref="D31:Q31"/>
+    <mergeCell ref="D32:Q32"/>
+    <mergeCell ref="D24:Q24"/>
+    <mergeCell ref="D25:Q25"/>
+    <mergeCell ref="D26:Q26"/>
+    <mergeCell ref="D27:Q27"/>
+    <mergeCell ref="D28:Q28"/>
+    <mergeCell ref="D29:Q29"/>
     <mergeCell ref="D23:Q23"/>
     <mergeCell ref="D3:Q3"/>
     <mergeCell ref="D11:Q11"/>
@@ -5503,15 +5500,15 @@
     <mergeCell ref="D20:Q20"/>
     <mergeCell ref="D21:Q21"/>
     <mergeCell ref="D22:Q22"/>
-    <mergeCell ref="D30:Q30"/>
-    <mergeCell ref="D31:Q31"/>
-    <mergeCell ref="D32:Q32"/>
-    <mergeCell ref="D24:Q24"/>
-    <mergeCell ref="D25:Q25"/>
-    <mergeCell ref="D26:Q26"/>
-    <mergeCell ref="D27:Q27"/>
-    <mergeCell ref="D28:Q28"/>
-    <mergeCell ref="D29:Q29"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="D13:Q13"/>
+    <mergeCell ref="D4:Q4"/>
+    <mergeCell ref="D5:Q5"/>
+    <mergeCell ref="D6:Q6"/>
+    <mergeCell ref="D7:Q7"/>
+    <mergeCell ref="D8:Q8"/>
+    <mergeCell ref="D9:Q9"/>
+    <mergeCell ref="D10:Q10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>